<commit_message>
DB - Adapting the configuration to changed names and folder structure refs #1065
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/sql/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/sql/template/User_Schema_Rights_Definition.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\INTERPOLAR\Postgres-cds_hub\init\template\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHub\INTERPOLAR\Postgres-cds_hub\sql\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -313,9 +313,6 @@
     <t>./R-cds2db/cds2db/inst/extdata/Table_Description.xlsx[table_description]</t>
   </si>
   <si>
-    <t>100_cre_table_raw_cds2db_in.sql</t>
-  </si>
-  <si>
     <t>template_cre_table.sql</t>
   </si>
   <si>
@@ -337,54 +334,33 @@
     <t>db_user</t>
   </si>
   <si>
-    <t>120_cre_table_raw_db_log.sql</t>
-  </si>
-  <si>
     <t>db_log_user</t>
   </si>
   <si>
     <t>db_log</t>
   </si>
   <si>
-    <t>300_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
     <t>template_copy_function.sql</t>
   </si>
   <si>
     <t>copy_raw_cds_in_to_db_log</t>
   </si>
   <si>
-    <t>140_cre_table_typ_cds2db_in.sql</t>
-  </si>
-  <si>
     <t>TYPED</t>
   </si>
   <si>
-    <t>150_get_last_processing_nr_typed.sql</t>
-  </si>
-  <si>
     <t>template_get_last_pnr_typed.sql</t>
   </si>
   <si>
     <t>get_last_processing_nr_typed</t>
   </si>
   <si>
-    <t>160_cre_table_typ_log.sql</t>
-  </si>
-  <si>
-    <t>310_cds_in_to_db_log.sql</t>
-  </si>
-  <si>
     <t>copy_type_cds_in_to_db_log</t>
   </si>
   <si>
     <t>SELECT</t>
   </si>
   <si>
-    <t>180_cre_view_raw_type_diff_log.sql</t>
-  </si>
-  <si>
     <t>template_cre_view_diff.sql</t>
   </si>
   <si>
@@ -397,9 +373,6 @@
     <t>_raw_diff</t>
   </si>
   <si>
-    <t>190_cre_view_typ_dataproc_all.sql</t>
-  </si>
-  <si>
     <t>template_cre_view_all.sql</t>
   </si>
   <si>
@@ -409,78 +382,42 @@
     <t>db2dataprocessor_out</t>
   </si>
   <si>
-    <t>190_cre_view_typ_dataproc_last_import.sql</t>
-  </si>
-  <si>
     <t>template_cre_view_last_import.sql</t>
   </si>
   <si>
     <t>_last_import</t>
   </si>
   <si>
-    <t>200_take_over_check_date.sql</t>
-  </si>
-  <si>
     <t>template_take_over_check_date_function.sql</t>
   </si>
   <si>
     <t>take_over_last_check_date</t>
   </si>
   <si>
-    <t>210_cre_view_typ_cds2db_all.sql</t>
-  </si>
-  <si>
-    <t>220_cre_view_raw_cds2db_last_import.sql</t>
-  </si>
-  <si>
     <t>_raw_last_import</t>
   </si>
   <si>
-    <t>230_cre_view_typ_cds2db_last_version.sql</t>
-  </si>
-  <si>
     <t>template_cre_view_last_version.sql</t>
   </si>
   <si>
     <t>_last_version</t>
   </si>
   <si>
-    <t>230_cre_view_raw_cds2db_last_version.sql</t>
-  </si>
-  <si>
     <t>_raw_last_version</t>
   </si>
   <si>
-    <t>230_cre_view_typ_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t>230_cre_view_raw_dataproc_last_version.sql</t>
-  </si>
-  <si>
-    <t>250_adding_historical_raw_records.sql</t>
-  </si>
-  <si>
     <t>template_adding_historical_records.sql</t>
   </si>
   <si>
-    <t>template_migration.sql</t>
-  </si>
-  <si>
     <t>./R-db2frontend/db2frontend/inst/extdata/Frontend_Table_Description.xlsx[frontend_table_description]</t>
   </si>
   <si>
-    <t>400_cre_table_typ_dataproc_in.sql</t>
-  </si>
-  <si>
     <t>db2dataprocessor_in</t>
   </si>
   <si>
     <t>_fe</t>
   </si>
   <si>
-    <t>440_cre_table_frontend_in.sql</t>
-  </si>
-  <si>
     <t>db2frontend_user</t>
   </si>
   <si>
@@ -490,87 +427,33 @@
     <t>INT_ID</t>
   </si>
   <si>
-    <t>420_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t>600_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
     <t>copy_fe_dp_in_to_db_log</t>
   </si>
   <si>
-    <t>430_cre_table_frontend_log.sql</t>
-  </si>
-  <si>
-    <t>620_fe_in_to_db_log.sql</t>
-  </si>
-  <si>
     <t>copy_fe_fe_in_to_db_log</t>
   </si>
   <si>
-    <t>520_cre_view_fe_out.sql</t>
-  </si>
-  <si>
     <t>db2frontend_out</t>
   </si>
   <si>
-    <t>450_cre_table_frontend_in_trig.sql</t>
-  </si>
-  <si>
     <t>template_cre_trigger_set_id.sql</t>
   </si>
   <si>
-    <t>460_cre_view_fe_dataproc_last_import.sql</t>
-  </si>
-  <si>
     <t>_fe_last_import</t>
   </si>
   <si>
-    <t>470_cre_view_fe_dataproc_all.sql</t>
-  </si>
-  <si>
     <t>./R-dataprocessor/submodules/Dataprocessor_Submodules_Table_Description.xlsx[table_description]</t>
   </si>
   <si>
-    <t>330_cre_table_dataproc_submodules_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t>331_cre_table_dataproc_submodules_log.sql</t>
-  </si>
-  <si>
-    <t>332_db_submodules_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
     <t>copy_submodules_dp_in_to_db_log</t>
   </si>
   <si>
-    <t>334_cre_view_dataproc_submodules_last_import.sql</t>
-  </si>
-  <si>
-    <t>335_cre_view_dataproc_submodules_all.sql</t>
-  </si>
-  <si>
     <t>./R-dataprocessor/dataprocessor/inst/extdata/Dataprocessor_Table_Description.xlsx[table_description]</t>
   </si>
   <si>
-    <t>340_cre_table_dataproc_core_dataproc_in.sql</t>
-  </si>
-  <si>
-    <t>341_cre_table_dataproc_core_log.sql</t>
-  </si>
-  <si>
-    <t>342_db_core_dp_in_to_db_log.sql</t>
-  </si>
-  <si>
     <t>copy_core_dp_in_to_db_log</t>
   </si>
   <si>
-    <t>344_cre_view_dataproc_core_last_import.sql</t>
-  </si>
-  <si>
-    <t>345_cre_view_dataproc_core_all.sql</t>
-  </si>
-  <si>
     <t>TABLE_DEFINITION</t>
   </si>
   <si>
@@ -664,16 +547,133 @@
     <t>template_cre_view_parameter.sql</t>
   </si>
   <si>
-    <t>031_cre_view_parameter_cds2db_out.sql</t>
-  </si>
-  <si>
-    <t>032_cre_view_parameter_dataproc_out.sql</t>
-  </si>
-  <si>
     <t>fix</t>
   </si>
   <si>
-    <t>033_cre_view_parameter_frontend_out.sql</t>
+    <t>base/031_cre_view_parameter_cds2db_out.sql</t>
+  </si>
+  <si>
+    <t>base/032_cre_view_parameter_dataproc_out.sql</t>
+  </si>
+  <si>
+    <t>base/033_cre_view_parameter_frontend_out.sql</t>
+  </si>
+  <si>
+    <t>base/100_cre_table_raw_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>base/120_cre_table_raw_db_log.sql</t>
+  </si>
+  <si>
+    <t>base/140_cre_table_typ_cds2db_in.sql</t>
+  </si>
+  <si>
+    <t>base/160_cre_table_typ_log.sql</t>
+  </si>
+  <si>
+    <t>base/180_cre_view_raw_type_diff_log.sql</t>
+  </si>
+  <si>
+    <t>base/190_cre_view_typ_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>base/190_cre_view_typ_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t>base/200_take_over_check_date.sql</t>
+  </si>
+  <si>
+    <t>base/210_cre_view_typ_cds2db_all.sql</t>
+  </si>
+  <si>
+    <t>base/220_cre_view_raw_cds2db_last_import.sql</t>
+  </si>
+  <si>
+    <t>base/230_cre_view_typ_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>base/230_cre_view_raw_cds2db_last_version.sql</t>
+  </si>
+  <si>
+    <t>base/230_cre_view_typ_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>base/230_cre_view_raw_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>base/250_adding_historical_raw_records.sql</t>
+  </si>
+  <si>
+    <t>base/400_cre_table_typ_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>base/440_cre_table_frontend_in.sql</t>
+  </si>
+  <si>
+    <t>base/420_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>base/430_cre_table_frontend_log.sql</t>
+  </si>
+  <si>
+    <t>base/520_cre_view_fe_out.sql</t>
+  </si>
+  <si>
+    <t>base/450_cre_table_frontend_in_trig.sql</t>
+  </si>
+  <si>
+    <t>base/460_cre_view_fe_dataproc_last_import.sql</t>
+  </si>
+  <si>
+    <t>base/470_cre_view_fe_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>base/330_cre_table_dataproc_submodules_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>base/331_cre_table_dataproc_submodules_log.sql</t>
+  </si>
+  <si>
+    <t>base/334_cre_view_dataproc_submodules_last_import.sql</t>
+  </si>
+  <si>
+    <t>base/335_cre_view_dataproc_submodules_all.sql</t>
+  </si>
+  <si>
+    <t>base/340_cre_table_dataproc_core_dataproc_in.sql</t>
+  </si>
+  <si>
+    <t>base/341_cre_table_dataproc_core_log.sql</t>
+  </si>
+  <si>
+    <t>base/344_cre_view_dataproc_core_last_import.sql</t>
+  </si>
+  <si>
+    <t>base/345_cre_view_dataproc_core_all.sql</t>
+  </si>
+  <si>
+    <t>template_start.sql</t>
+  </si>
+  <si>
+    <t>base/300_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>base/150_get_last_processing_nr_typed.sql</t>
+  </si>
+  <si>
+    <t>base/310_cds_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>base/600_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>base/620_fe_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>base/332_db_submodules_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>base/342_db_core_dp_in_to_db_log.sql</t>
   </si>
 </sst>
 </file>
@@ -1057,8 +1057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1195,7 +1195,7 @@
         <v>21</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
@@ -1264,1190 +1264,1190 @@
         <v>29</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>147</v>
+        <v>109</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F24" s="6"/>
       <c r="G24" s="6" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="H24" s="6"/>
       <c r="I24" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J24" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>148</v>
+        <v>110</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F25" s="6"/>
       <c r="G25" s="6" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>150</v>
+        <v>111</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>146</v>
+        <v>107</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="F26" s="6"/>
       <c r="G26" s="6" t="s">
-        <v>149</v>
+        <v>108</v>
       </c>
       <c r="H26" s="6"/>
       <c r="I26" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="D27" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F27" s="1" t="s">
+      <c r="H27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="I27" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I27" s="1" t="s">
-        <v>36</v>
-      </c>
       <c r="J27" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I28" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J28" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="J28" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D29" s="1" t="s">
+      <c r="F29" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="N29" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O29" s="1" t="s">
         <v>34</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I29" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="M29" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="N29" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="O29" s="1" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J30" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="J30" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="C31" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F31" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>46</v>
+        <v>145</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="I32" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J32" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="33" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B33" s="6" t="s">
-        <v>49</v>
+        <v>115</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D33" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="I33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>146</v>
+      </c>
+      <c r="L33" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="I33" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J33" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K33" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="L33" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="M33" s="6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="N33" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B34" s="6"/>
       <c r="I34" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J34" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="J34" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="35" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B35" s="6"/>
       <c r="I35" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J35" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B36" s="6" t="s">
-        <v>53</v>
+        <v>116</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="I36" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J36" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N36" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O36" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="P36" s="8"/>
     </row>
     <row r="37" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B37" s="6"/>
       <c r="I37" s="7" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J37" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B38" s="6" t="s">
-        <v>58</v>
+        <v>117</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E38" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J38" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N38" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="39" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B39" s="6" t="s">
-        <v>62</v>
+        <v>118</v>
       </c>
       <c r="C39" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D39" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J39" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N39" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B40" s="6" t="s">
-        <v>65</v>
+        <v>119</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K40" s="6" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="M40" s="6" t="s">
-        <v>67</v>
+        <v>56</v>
       </c>
       <c r="N40" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B41" s="6" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D41" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J41" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N41" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="42" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B42" s="6" t="s">
-        <v>69</v>
+        <v>121</v>
       </c>
       <c r="C42" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D42" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J42" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N42" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O42" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="43" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B43" s="6" t="s">
-        <v>71</v>
+        <v>122</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F43" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G43" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I43" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I43" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="J43" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="N43" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="44" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B44" s="6" t="s">
-        <v>74</v>
+        <v>123</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D44" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="F44" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G44" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I44" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J44" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N44" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O44" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="G44" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H44" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I44" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J44" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="N44" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O44" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="45" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B45" s="6" t="s">
-        <v>76</v>
+        <v>124</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D45" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="F45" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I45" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="G45" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H45" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="I45" s="6" t="s">
-        <v>52</v>
-      </c>
       <c r="J45" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B46" s="6" t="s">
-        <v>77</v>
+        <v>125</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D46" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H46" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F46" s="6" t="s">
+      <c r="I46" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N46" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O46" s="6" t="s">
         <v>34</v>
-      </c>
-      <c r="G46" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H46" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="I46" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J46" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="N46" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O46" s="6" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="47" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B47" s="6" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="D47" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="J47" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="N47" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="E47" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="G47" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="J47" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="N47" s="6" t="s">
-        <v>33</v>
-      </c>
       <c r="O47" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B48" s="6" t="str">
-        <f>"migration/migration.sql"</f>
-        <v>migration/migration.sql</v>
+        <f>"start.sql"</f>
+        <v>start.sql</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>80</v>
+        <v>143</v>
       </c>
       <c r="J48" s="7"/>
     </row>
     <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>81</v>
+        <v>62</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>82</v>
+        <v>127</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B50" s="10"/>
       <c r="I50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J50" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="J50" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I51" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="I53" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="J53" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="J53" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C54" s="11"/>
       <c r="I54" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J54" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
-        <v>89</v>
+        <v>129</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D55" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I55" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K55" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="L55" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E55" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F55" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H55" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I55" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K55" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="L55" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="M55" s="6" t="s">
-        <v>91</v>
+        <v>68</v>
       </c>
       <c r="N55" s="6" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="O55" s="6" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B56" s="6"/>
       <c r="C56" s="11"/>
       <c r="J56" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B57" s="6" t="s">
-        <v>92</v>
+        <v>130</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D57" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E57" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H57" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I57" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J57" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K57" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="L57" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="E57" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>145</v>
-      </c>
-      <c r="H57" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="I57" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="J57" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="K57" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="L57" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="M57" s="6" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="N57" s="6" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="O57" s="6" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B58" s="6"/>
       <c r="C58" s="11"/>
       <c r="I58" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J58" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="J58" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B59" s="6" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D59" s="6" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="G59" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="I59" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J59" s="6" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="N59" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O59" s="6" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B60" s="6"/>
       <c r="C60" s="11"/>
       <c r="I60" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J60" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B61" s="6" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>98</v>
+        <v>71</v>
       </c>
       <c r="D61" s="6" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="62" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B62" s="6" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="C62" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D62" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G62" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H62" s="6" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="I62" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J62" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N62" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O62" s="6" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B63" s="6" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G63" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H63" s="6" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="I63" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J63" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N63" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="O63" s="6" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>102</v>
+        <v>73</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>103</v>
+        <v>135</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B65" s="6"/>
       <c r="I65" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J65" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I66" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B67" s="1" t="s">
-        <v>104</v>
+        <v>136</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D67" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F67" s="6" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="H67" s="6"/>
       <c r="I67" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J67" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K67" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="L67" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K67" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="L67" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="M67" s="6" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
       <c r="N67" s="6" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B68" s="6"/>
       <c r="C68" s="11"/>
       <c r="J68" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B69" s="6" t="s">
-        <v>107</v>
+        <v>137</v>
       </c>
       <c r="C69" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D69" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E69" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G69" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H69" s="6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="I69" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J69" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N69" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B70" s="6" t="s">
-        <v>108</v>
+        <v>138</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D70" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H70" s="6"/>
       <c r="I70" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N70" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>109</v>
+        <v>75</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>110</v>
+        <v>139</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="I71" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
       <c r="I72" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J72" s="6" t="s">
         <v>36</v>
-      </c>
-      <c r="J72" s="6" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I73" s="1" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B74" s="1" t="s">
-        <v>111</v>
+        <v>140</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="H74" s="6"/>
       <c r="I74" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J74" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K74" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="L74" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="K74" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="L74" s="6" t="s">
-        <v>42</v>
-      </c>
       <c r="M74" s="6" t="s">
-        <v>113</v>
+        <v>76</v>
       </c>
       <c r="N74" s="6" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B75" s="6"/>
       <c r="C75" s="11"/>
       <c r="J75" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B76" s="6" t="s">
-        <v>114</v>
+        <v>141</v>
       </c>
       <c r="C76" s="9" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="D76" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G76" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H76" s="6" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="I76" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J76" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N76" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B77" s="6" t="s">
-        <v>115</v>
+        <v>142</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="D77" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G77" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="H77" s="6"/>
       <c r="I77" s="6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="J77" s="6" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="N77" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -2489,42 +2489,42 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>116</v>
+        <v>77</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>117</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>119</v>
+        <v>80</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>121</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>123</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>125</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2537,16 +2537,16 @@
         <v>3</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>118</v>
+        <v>79</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>120</v>
+        <v>81</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>122</v>
+        <v>83</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2554,90 +2554,90 @@
         <v>29</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>129</v>
+        <v>90</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>128</v>
+        <v>89</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>131</v>
+        <v>92</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>132</v>
+        <v>93</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>133</v>
+        <v>94</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>134</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>135</v>
+        <v>96</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>137</v>
+        <v>98</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>138</v>
+        <v>99</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>139</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D16" s="1" t="s">
-        <v>140</v>
+        <v>101</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>141</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D17" s="1" t="s">
-        <v>142</v>
+        <v>103</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>143</v>
+        <v>104</v>
       </c>
     </row>
     <row r="18" spans="4:5" x14ac:dyDescent="0.25">
       <c r="D18" s="1" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>144</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DB - Renaming the scripts for views for the data processor, configuring the new views for the frontend refs #1138
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/sql/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/sql/template/User_Schema_Rights_Definition.xlsx
@@ -170,7 +170,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K67" authorId="0" shapeId="0">
+    <comment ref="K71" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +193,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K74" authorId="0" shapeId="0">
+    <comment ref="K78" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -221,7 +221,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="155">
   <si>
     <t>Erklärung</t>
   </si>
@@ -625,9 +625,6 @@
     <t>base/460_cre_view_fe_dataproc_last_import.sql</t>
   </si>
   <si>
-    <t>base/470_cre_view_fe_dataproc_all.sql</t>
-  </si>
-  <si>
     <t>base/330_cre_table_dataproc_submodules_dataproc_in.sql</t>
   </si>
   <si>
@@ -674,6 +671,21 @@
   </si>
   <si>
     <t>base/342_db_core_dp_in_to_db_log.sql</t>
+  </si>
+  <si>
+    <t>base/461_cre_view_fe_dataproc_all.sql</t>
+  </si>
+  <si>
+    <t>base/462_cre_view_fe_dataproc_last_version.sql</t>
+  </si>
+  <si>
+    <t>base/470_cre_view_fe_frontend_last_import.sql</t>
+  </si>
+  <si>
+    <t>base/471_cre_view_fe_frontend_all.sql</t>
+  </si>
+  <si>
+    <t>base/472_cre_view_fe_frontend_last_version.sql</t>
   </si>
 </sst>
 </file>
@@ -1055,10 +1067,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q77"/>
+  <dimension ref="A1:Q81"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="J61" sqref="J61"/>
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1397,7 +1409,7 @@
         <v>37</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="L29" s="1" t="s">
         <v>39</v>
@@ -1443,7 +1455,7 @@
         <v>31</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="L31" s="1" t="s">
         <v>42</v>
@@ -1486,7 +1498,7 @@
         <v>37</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L33" s="6" t="s">
         <v>39</v>
@@ -1863,7 +1875,7 @@
         <v>start.sql</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J48" s="7"/>
     </row>
@@ -1979,7 +1991,7 @@
         <v>37</v>
       </c>
       <c r="K55" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="L55" s="6" t="s">
         <v>39</v>
@@ -2027,7 +2039,7 @@
         <v>37</v>
       </c>
       <c r="K57" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="L57" s="6" t="s">
         <v>39</v>
@@ -2142,7 +2154,7 @@
     </row>
     <row r="63" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B63" s="6" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="C63" s="6" t="s">
         <v>50</v>
@@ -2173,280 +2185,410 @@
       </c>
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
+      <c r="B64" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E64" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H64" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I64" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J64" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N64" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O64" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="65" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B65" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C65" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E65" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G65" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="I65" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J65" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N65" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O65" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B66" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E66" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G66" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="I66" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N66" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O66" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B67" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H67" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="I67" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="N67" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O67" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B68" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I68" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J68" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B69" s="6"/>
+      <c r="I69" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J69" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I70" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B71" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C71" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D64" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E64" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I64" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J64" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B65" s="6"/>
-      <c r="I65" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J65" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I66" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J66" s="1" t="s">
+      <c r="D71" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B67" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F67" s="6" t="s">
+      <c r="E71" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F71" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="H67" s="6"/>
-      <c r="I67" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K67" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="L67" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M67" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="N67" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B68" s="6"/>
-      <c r="C68" s="11"/>
-      <c r="J68" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B69" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C69" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D69" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I69" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N69" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B70" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C70" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E70" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G70" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J70" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N70" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A71" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B71" s="6" t="s">
-        <v>139</v>
-      </c>
-      <c r="C71" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>63</v>
-      </c>
+      <c r="H71" s="6"/>
       <c r="I71" s="6" t="s">
         <v>35</v>
       </c>
       <c r="J71" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="K71" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="L71" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M71" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N71" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B72" s="6"/>
-      <c r="I72" s="6" t="s">
-        <v>35</v>
-      </c>
+      <c r="C72" s="11"/>
       <c r="J72" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="I73" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="J73" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B74" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="C74" s="11" t="s">
-        <v>30</v>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B73" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D73" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E73" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G73" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H73" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I73" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J73" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N73" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B74" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C74" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="D74" s="6" t="s">
-        <v>37</v>
+        <v>51</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>67</v>
+        <v>52</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>48</v>
       </c>
       <c r="H74" s="6"/>
       <c r="I74" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N74" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A75" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C75" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E75" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="I75" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="J74" s="6" t="s">
+      <c r="J75" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B76" s="6"/>
+      <c r="I76" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J76" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I77" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J77" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="K74" s="6" t="s">
-        <v>150</v>
-      </c>
-      <c r="L74" s="6" t="s">
+    </row>
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B78" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F78" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J78" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K78" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="L78" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="M74" s="6" t="s">
+      <c r="M78" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="N74" s="6" t="s">
+      <c r="N78" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B75" s="6"/>
-      <c r="C75" s="11"/>
-      <c r="J75" s="6" t="s">
+    <row r="79" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B79" s="6"/>
+      <c r="C79" s="11"/>
+      <c r="J79" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B76" s="6" t="s">
+    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B80" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C80" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D80" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E80" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G80" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H80" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I80" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J80" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N80" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="B81" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="C76" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D76" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E76" s="6" t="s">
+      <c r="C81" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E81" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G76" s="6" t="s">
+      <c r="G81" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="H76" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I76" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J76" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N76" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="B77" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E77" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G77" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J77" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N77" s="6" t="s">
+      <c r="H81" s="6"/>
+      <c r="I81" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J81" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N81" s="6" t="s">
         <v>38</v>
       </c>
     </row>

</xml_diff>

<commit_message>
DB - Generation of view scripts and manual creation of last_version - adjustment of the configuration table refs #1138
</commit_message>
<xml_diff>
--- a/Postgres-cds_hub/sql/template/User_Schema_Rights_Definition.xlsx
+++ b/Postgres-cds_hub/sql/template/User_Schema_Rights_Definition.xlsx
@@ -14,6 +14,7 @@
   <sheets>
     <sheet name="rights_and_functions" sheetId="1" r:id="rId1"/>
     <sheet name="table_description_convert_def" sheetId="2" r:id="rId2"/>
+    <sheet name="noch_manuel_generierung_umsetze" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -170,7 +171,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K71" authorId="0" shapeId="0">
+    <comment ref="K69" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -193,7 +194,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K78" authorId="0" shapeId="0">
+    <comment ref="K76" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -220,8 +221,66 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Unbekannter Autor</author>
+  </authors>
+  <commentList>
+    <comment ref="D2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Autor:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>GRANT TRIGGER
+GRANT USAGE ON SCHEMA
+GRANT USAGE ON seq</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Autor:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Segoe UI"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rawdaten = varchar oder kein Eintrag dann Datentypen</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="156">
   <si>
     <t>Erklärung</t>
   </si>
@@ -686,6 +745,9 @@
   </si>
   <si>
     <t>base/472_cre_view_fe_frontend_last_version.sql</t>
+  </si>
+  <si>
+    <t>_fe_last_version</t>
   </si>
 </sst>
 </file>
@@ -1067,10 +1129,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q81"/>
+  <dimension ref="A1:Q79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A66" sqref="A66"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B65" sqref="B65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,29 +2248,28 @@
     </row>
     <row r="64" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B64" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="C64" s="6" t="s">
-        <v>58</v>
+        <v>152</v>
+      </c>
+      <c r="C64" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="D64" s="6" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="F64" s="6"/>
+        <v>70</v>
+      </c>
       <c r="G64" s="6" t="s">
         <v>48</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="I64" s="6" t="s">
         <v>45</v>
       </c>
       <c r="J64" s="6" t="s">
-        <v>51</v>
+        <v>65</v>
       </c>
       <c r="N64" s="6" t="s">
         <v>38</v>
@@ -2219,10 +2280,10 @@
     </row>
     <row r="65" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B65" s="6" t="s">
-        <v>152</v>
-      </c>
-      <c r="C65" s="9" t="s">
-        <v>53</v>
+        <v>153</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>50</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>65</v>
@@ -2234,7 +2295,7 @@
         <v>48</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I65" s="6" t="s">
         <v>45</v>
@@ -2250,345 +2311,280 @@
       </c>
     </row>
     <row r="66" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="B66" s="6" t="s">
-        <v>153</v>
+        <v>134</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="D66" s="6" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="G66" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="I66" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J66" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B67" s="6"/>
+      <c r="I67" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J67" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I68" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J66" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="N66" s="6" t="s">
+      <c r="J68" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B69" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E69" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="O66" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="67" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B67" s="6" t="s">
-        <v>154</v>
-      </c>
-      <c r="C67" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D67" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="E67" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="F67" s="6"/>
-      <c r="G67" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H67" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="I67" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="N67" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="O67" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="68" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="B68" s="6" t="s">
-        <v>134</v>
-      </c>
-      <c r="C68" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D68" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E68" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I68" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="69" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B69" s="6"/>
+      <c r="F69" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H69" s="6"/>
       <c r="I69" s="6" t="s">
         <v>35</v>
       </c>
       <c r="J69" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K69" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="L69" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M69" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="N69" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B70" s="6"/>
+      <c r="C70" s="11"/>
+      <c r="J70" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="70" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I70" s="1" t="s">
+    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B71" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D71" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E71" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G71" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H71" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I71" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J70" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="71" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B71" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C71" s="11" t="s">
+      <c r="J71" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N71" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B72" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="C72" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D72" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E72" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G72" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J72" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N72" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A73" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B73" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="C73" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E71" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J71" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K71" s="6" t="s">
-        <v>148</v>
-      </c>
-      <c r="L71" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M71" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="N71" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="72" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B72" s="6"/>
-      <c r="C72" s="11"/>
-      <c r="J72" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="73" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B73" s="6" t="s">
-        <v>136</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>53</v>
       </c>
       <c r="D73" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G73" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H73" s="6" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="J73" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="N73" s="6" t="s">
+    </row>
+    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B74" s="6"/>
+      <c r="I74" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J74" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I75" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J75" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B76" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="C76" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E76" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="74" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B74" s="6" t="s">
-        <v>137</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D74" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E74" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G74" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J74" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N74" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="75" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A75" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="B75" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E75" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="I75" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J75" s="6" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="76" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B76" s="6"/>
+      <c r="F76" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H76" s="6"/>
       <c r="I76" s="6" t="s">
         <v>35</v>
       </c>
       <c r="J76" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="K76" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="L76" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="M76" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="N76" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B77" s="6"/>
+      <c r="C77" s="11"/>
+      <c r="J77" s="6" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="77" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="I77" s="1" t="s">
+    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B78" s="6" t="s">
+        <v>140</v>
+      </c>
+      <c r="C78" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E78" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H78" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="I78" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="J77" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="78" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B78" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C78" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D78" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E78" s="6" t="s">
+      <c r="J78" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="N78" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="F78" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="J78" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="K78" s="6" t="s">
-        <v>149</v>
-      </c>
-      <c r="L78" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="M78" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="N78" s="6" t="s">
-        <v>63</v>
-      </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B79" s="6"/>
-      <c r="C79" s="11"/>
+      <c r="B79" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G79" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6" t="s">
+        <v>45</v>
+      </c>
       <c r="J79" s="6" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="80" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B80" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="C80" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="D80" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="E80" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G80" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H80" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I80" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J80" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N80" s="6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="81" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B81" s="6" t="s">
-        <v>141</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="E81" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G81" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="J81" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N81" s="6" t="s">
+      <c r="N79" s="6" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2786,4 +2782,189 @@
   <pageMargins left="0.7" right="0.7" top="0.78749999999999998" bottom="0.78749999999999998" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="97.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="1"/>
+      <c r="P1" s="1"/>
+      <c r="Q1" s="1"/>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>151</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="6" t="s">
+        <v>154</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>155</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>